<commit_message>
add type attribute column for Compartment
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/2_species_1_reaction.xlsx
+++ b/tests/multialgorithm/fixtures/2_species_1_reaction.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_sim/tests/multialgorithm/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/wc_sim/tests/multialgorithm/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="37900" windowHeight="21140" tabRatio="989" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="37900" windowHeight="21140" tabRatio="989" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10">'Biomass components'!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11">'Biomass reactions'!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3">Compartments!$A$1:$F$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3">Compartments!$A$1:$G$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">Concentrations!$A$1:$E$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15">'Database references'!$A$1:$J$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7">Functions!$A$1:$E$1</definedName>
@@ -47,7 +47,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2">Submodels!$A$1:$I$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">Taxon!$A$1:$A$6</definedName>
   </definedNames>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="78">
   <si>
     <t>Id</t>
   </si>
@@ -779,7 +779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1298,18 +1298,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1323,13 +1323,16 @@
         <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -1344,9 +1347,10 @@
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F2"/>
+  <autoFilter ref="A1:G2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>